<commit_message>
added Test case 31,32
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Netology\Qa-Diplom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18B74CD-DB64-488E-AAA1-B26FF86AD966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6B0AD6-BE3D-41A4-91D8-9EE2F9E12405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="215">
   <si>
     <t>ID</t>
   </si>
@@ -652,6 +652,24 @@
   </si>
   <si>
     <t>2. Приложение исчезло из активных</t>
+  </si>
+  <si>
+    <t>Добавление новой новости с некорректным временем</t>
+  </si>
+  <si>
+    <t>6. В поле "Время" набрать с помощью клавиатуры некорректное время новости 25 00 и нажать ок</t>
+  </si>
+  <si>
+    <t>6. Некорректное время не вводится в поле, возникает предупреждение, что необходимо ввести корректные данные</t>
+  </si>
+  <si>
+    <t>Добавление новой новости с некорректой датой из прошлого</t>
+  </si>
+  <si>
+    <t>5. В поле "Дата" выбрать некорректное значение из прошлого</t>
+  </si>
+  <si>
+    <t>5. Некорректная дата не вводится в поле, возникает предупреждение, что необходимо ввести корректные данные</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1268,22 +1286,145 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1292,27 +1433,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1320,112 +1440,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1775,10 +1802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K136"/>
+  <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C11"/>
+    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E138" sqref="E138:E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1824,19 +1851,19 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="58">
+      <c r="A2" s="86">
         <v>1</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="60" t="s">
+      <c r="D2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F2" s="10" t="s">
@@ -1846,16 +1873,16 @@
         <v>11</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="77" t="s">
+      <c r="I2" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58"/>
-      <c r="B3" s="78"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
       <c r="F3" s="12" t="s">
         <v>13</v>
       </c>
@@ -1863,14 +1890,14 @@
         <v>14</v>
       </c>
       <c r="H3" s="13"/>
-      <c r="I3" s="77"/>
+      <c r="I3" s="99"/>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58"/>
-      <c r="B4" s="78"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
+      <c r="A4" s="86"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
       <c r="F4" s="12" t="s">
         <v>15</v>
       </c>
@@ -1878,14 +1905,14 @@
         <v>16</v>
       </c>
       <c r="H4" s="13"/>
-      <c r="I4" s="77"/>
+      <c r="I4" s="99"/>
     </row>
     <row r="5" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="58"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="14" t="s">
         <v>17</v>
       </c>
@@ -1893,22 +1920,22 @@
         <v>18</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="77"/>
+      <c r="I5" s="99"/>
     </row>
     <row r="6" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="58">
+      <c r="A6" s="86">
         <v>2</v>
       </c>
-      <c r="B6" s="78" t="s">
+      <c r="B6" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="60" t="s">
+      <c r="C6" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F6" s="10" t="s">
@@ -1918,16 +1945,16 @@
         <v>11</v>
       </c>
       <c r="H6" s="11"/>
-      <c r="I6" s="77" t="s">
+      <c r="I6" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
-      <c r="B7" s="78"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
+      <c r="A7" s="86"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
       <c r="F7" s="12" t="s">
         <v>13</v>
       </c>
@@ -1935,14 +1962,14 @@
         <v>14</v>
       </c>
       <c r="H7" s="13"/>
-      <c r="I7" s="77"/>
+      <c r="I7" s="99"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="58"/>
-      <c r="B8" s="78"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
+      <c r="A8" s="86"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
       <c r="F8" s="12" t="s">
         <v>15</v>
       </c>
@@ -1950,14 +1977,14 @@
         <v>16</v>
       </c>
       <c r="H8" s="13"/>
-      <c r="I8" s="77"/>
+      <c r="I8" s="99"/>
     </row>
     <row r="9" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
-      <c r="B9" s="78"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
+      <c r="A9" s="86"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
       <c r="F9" s="12" t="s">
         <v>17</v>
       </c>
@@ -1965,14 +1992,14 @@
         <v>18</v>
       </c>
       <c r="H9" s="13"/>
-      <c r="I9" s="77"/>
+      <c r="I9" s="99"/>
     </row>
     <row r="10" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="78"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
+      <c r="A10" s="86"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
       <c r="F10" s="12" t="s">
         <v>20</v>
       </c>
@@ -1980,14 +2007,14 @@
         <v>21</v>
       </c>
       <c r="H10" s="13"/>
-      <c r="I10" s="77"/>
+      <c r="I10" s="99"/>
     </row>
     <row r="11" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="58"/>
-      <c r="B11" s="78"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
+      <c r="A11" s="86"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="62"/>
       <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
@@ -1995,22 +2022,22 @@
         <v>23</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="77"/>
+      <c r="I11" s="99"/>
     </row>
     <row r="12" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="58">
+      <c r="A12" s="86">
         <v>3</v>
       </c>
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="60" t="s">
+      <c r="C12" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="60" t="s">
+      <c r="E12" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F12" s="10" t="s">
@@ -2020,16 +2047,16 @@
         <v>11</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="77" t="s">
+      <c r="I12" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="58"/>
-      <c r="B13" s="78"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="60"/>
+      <c r="A13" s="86"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="62"/>
       <c r="F13" s="12" t="s">
         <v>93</v>
       </c>
@@ -2037,14 +2064,14 @@
         <v>26</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="77"/>
+      <c r="I13" s="99"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="58"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="60"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="62"/>
       <c r="F14" s="12" t="s">
         <v>27</v>
       </c>
@@ -2052,14 +2079,14 @@
         <v>28</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="77"/>
+      <c r="I14" s="99"/>
     </row>
     <row r="15" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="58"/>
-      <c r="B15" s="78"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="72"/>
-      <c r="E15" s="60"/>
+      <c r="A15" s="86"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="62"/>
       <c r="F15" s="14" t="s">
         <v>17</v>
       </c>
@@ -2067,22 +2094,22 @@
         <v>29</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="77"/>
+      <c r="I15" s="99"/>
     </row>
     <row r="16" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="58">
+      <c r="A16" s="86">
         <v>4</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="E16" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F16" s="10" t="s">
@@ -2092,16 +2119,16 @@
         <v>11</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="77" t="s">
+      <c r="I16" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="60"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="62"/>
       <c r="F17" s="12" t="s">
         <v>31</v>
       </c>
@@ -2109,14 +2136,14 @@
         <v>14</v>
       </c>
       <c r="H17" s="13"/>
-      <c r="I17" s="77"/>
+      <c r="I17" s="99"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="58"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="60"/>
+      <c r="A18" s="86"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="100"/>
+      <c r="E18" s="62"/>
       <c r="F18" s="12" t="s">
         <v>15</v>
       </c>
@@ -2124,14 +2151,14 @@
         <v>16</v>
       </c>
       <c r="H18" s="13"/>
-      <c r="I18" s="77"/>
+      <c r="I18" s="99"/>
     </row>
     <row r="19" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="78"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="60"/>
+      <c r="A19" s="86"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="100"/>
+      <c r="E19" s="62"/>
       <c r="F19" s="14" t="s">
         <v>17</v>
       </c>
@@ -2139,22 +2166,22 @@
         <v>32</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="77"/>
+      <c r="I19" s="99"/>
     </row>
     <row r="20" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="58">
+      <c r="A20" s="86">
         <v>5</v>
       </c>
-      <c r="B20" s="78" t="s">
+      <c r="B20" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F20" s="10" t="s">
@@ -2164,16 +2191,16 @@
         <v>11</v>
       </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="77" t="s">
+      <c r="I20" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
-      <c r="B21" s="78"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="60"/>
+      <c r="A21" s="86"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="100"/>
+      <c r="E21" s="62"/>
       <c r="F21" s="12" t="s">
         <v>13</v>
       </c>
@@ -2181,14 +2208,14 @@
         <v>14</v>
       </c>
       <c r="H21" s="13"/>
-      <c r="I21" s="77"/>
+      <c r="I21" s="99"/>
     </row>
     <row r="22" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="58"/>
-      <c r="B22" s="78"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="60"/>
+      <c r="A22" s="86"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="100"/>
+      <c r="E22" s="62"/>
       <c r="F22" s="12" t="s">
         <v>34</v>
       </c>
@@ -2196,14 +2223,14 @@
         <v>16</v>
       </c>
       <c r="H22" s="13"/>
-      <c r="I22" s="77"/>
+      <c r="I22" s="99"/>
     </row>
     <row r="23" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="58"/>
-      <c r="B23" s="78"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="72"/>
-      <c r="E23" s="60"/>
+      <c r="A23" s="86"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="62"/>
       <c r="F23" s="14" t="s">
         <v>17</v>
       </c>
@@ -2211,22 +2238,22 @@
         <v>32</v>
       </c>
       <c r="H23" s="15"/>
-      <c r="I23" s="77"/>
+      <c r="I23" s="99"/>
     </row>
     <row r="24" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="58">
+      <c r="A24" s="86">
         <v>6</v>
       </c>
-      <c r="B24" s="78" t="s">
+      <c r="B24" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="60" t="s">
+      <c r="D24" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F24" s="10" t="s">
@@ -2236,16 +2263,16 @@
         <v>11</v>
       </c>
       <c r="H24" s="11"/>
-      <c r="I24" s="77" t="s">
+      <c r="I24" s="99" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="58"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
       <c r="F25" s="12" t="s">
         <v>38</v>
       </c>
@@ -2253,14 +2280,14 @@
         <v>14</v>
       </c>
       <c r="H25" s="13"/>
-      <c r="I25" s="77"/>
+      <c r="I25" s="99"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="58"/>
-      <c r="B26" s="78"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
+      <c r="A26" s="86"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
       <c r="F26" s="12" t="s">
         <v>15</v>
       </c>
@@ -2268,14 +2295,14 @@
         <v>16</v>
       </c>
       <c r="H26" s="13"/>
-      <c r="I26" s="77"/>
+      <c r="I26" s="99"/>
     </row>
     <row r="27" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="58"/>
-      <c r="B27" s="78"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
+      <c r="A27" s="86"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
       <c r="F27" s="14" t="s">
         <v>17</v>
       </c>
@@ -2283,22 +2310,22 @@
         <v>39</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="77"/>
+      <c r="I27" s="99"/>
     </row>
     <row r="28" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="58">
+      <c r="A28" s="86">
         <v>7</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="60" t="s">
+      <c r="C28" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="60" t="s">
+      <c r="D28" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="60" t="s">
+      <c r="E28" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F28" s="10" t="s">
@@ -2308,16 +2335,16 @@
         <v>11</v>
       </c>
       <c r="H28" s="11"/>
-      <c r="I28" s="77" t="s">
+      <c r="I28" s="99" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="58"/>
-      <c r="B29" s="78"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
+      <c r="A29" s="86"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
       <c r="F29" s="12" t="s">
         <v>41</v>
       </c>
@@ -2325,14 +2352,14 @@
         <v>14</v>
       </c>
       <c r="H29" s="13"/>
-      <c r="I29" s="77"/>
+      <c r="I29" s="99"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="58"/>
-      <c r="B30" s="78"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
+      <c r="A30" s="86"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
       <c r="F30" s="12" t="s">
         <v>15</v>
       </c>
@@ -2340,14 +2367,14 @@
         <v>16</v>
       </c>
       <c r="H30" s="13"/>
-      <c r="I30" s="77"/>
+      <c r="I30" s="99"/>
     </row>
     <row r="31" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="58"/>
-      <c r="B31" s="78"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
+      <c r="A31" s="86"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
       <c r="F31" s="14" t="s">
         <v>17</v>
       </c>
@@ -2355,22 +2382,22 @@
         <v>39</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="77"/>
+      <c r="I31" s="99"/>
     </row>
     <row r="32" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="58">
+      <c r="A32" s="86">
         <v>8</v>
       </c>
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="60" t="s">
+      <c r="C32" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="60" t="s">
+      <c r="D32" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F32" s="10" t="s">
@@ -2380,16 +2407,16 @@
         <v>11</v>
       </c>
       <c r="H32" s="11"/>
-      <c r="I32" s="77" t="s">
+      <c r="I32" s="99" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="58"/>
-      <c r="B33" s="78"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
+      <c r="A33" s="86"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
       <c r="F33" s="12" t="s">
         <v>13</v>
       </c>
@@ -2397,14 +2424,14 @@
         <v>14</v>
       </c>
       <c r="H33" s="13"/>
-      <c r="I33" s="77"/>
+      <c r="I33" s="99"/>
     </row>
     <row r="34" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="58"/>
-      <c r="B34" s="78"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
+      <c r="A34" s="86"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
       <c r="F34" s="12" t="s">
         <v>43</v>
       </c>
@@ -2412,14 +2439,14 @@
         <v>16</v>
       </c>
       <c r="H34" s="13"/>
-      <c r="I34" s="77"/>
+      <c r="I34" s="99"/>
     </row>
     <row r="35" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="58"/>
-      <c r="B35" s="78"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
+      <c r="A35" s="86"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
       <c r="F35" s="14" t="s">
         <v>17</v>
       </c>
@@ -2427,22 +2454,22 @@
         <v>39</v>
       </c>
       <c r="H35" s="15"/>
-      <c r="I35" s="77"/>
+      <c r="I35" s="99"/>
     </row>
     <row r="36" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="58">
+      <c r="A36" s="86">
         <v>9</v>
       </c>
-      <c r="B36" s="78" t="s">
+      <c r="B36" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="60" t="s">
+      <c r="C36" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="60" t="s">
+      <c r="D36" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="60" t="s">
+      <c r="E36" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F36" s="10" t="s">
@@ -2452,16 +2479,16 @@
         <v>11</v>
       </c>
       <c r="H36" s="11"/>
-      <c r="I36" s="77" t="s">
+      <c r="I36" s="99" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="58"/>
-      <c r="B37" s="78"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
+      <c r="A37" s="86"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="62"/>
+      <c r="E37" s="62"/>
       <c r="F37" s="12" t="s">
         <v>13</v>
       </c>
@@ -2469,14 +2496,14 @@
         <v>14</v>
       </c>
       <c r="H37" s="13"/>
-      <c r="I37" s="77"/>
+      <c r="I37" s="99"/>
     </row>
     <row r="38" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="58"/>
-      <c r="B38" s="78"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
+      <c r="A38" s="86"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="62"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12" t="s">
         <v>45</v>
       </c>
@@ -2484,14 +2511,14 @@
         <v>16</v>
       </c>
       <c r="H38" s="13"/>
-      <c r="I38" s="77"/>
+      <c r="I38" s="99"/>
     </row>
     <row r="39" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="58"/>
-      <c r="B39" s="78"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
+      <c r="A39" s="86"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="62"/>
       <c r="F39" s="14" t="s">
         <v>17</v>
       </c>
@@ -2499,22 +2526,22 @@
         <v>39</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="77"/>
+      <c r="I39" s="99"/>
     </row>
     <row r="40" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="58">
+      <c r="A40" s="86">
         <v>10</v>
       </c>
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="81" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="60" t="s">
+      <c r="C40" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="60" t="s">
+      <c r="D40" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="60" t="s">
+      <c r="E40" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F40" s="10" t="s">
@@ -2524,16 +2551,16 @@
         <v>49</v>
       </c>
       <c r="H40" s="11"/>
-      <c r="I40" s="77" t="s">
+      <c r="I40" s="99" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="58"/>
-      <c r="B41" s="78"/>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
+      <c r="A41" s="86"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
       <c r="F41" s="12" t="s">
         <v>50</v>
       </c>
@@ -2541,14 +2568,14 @@
         <v>51</v>
       </c>
       <c r="H41" s="13"/>
-      <c r="I41" s="77"/>
+      <c r="I41" s="99"/>
     </row>
     <row r="42" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="58"/>
-      <c r="B42" s="78"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
+      <c r="A42" s="86"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
       <c r="F42" s="12" t="s">
         <v>52</v>
       </c>
@@ -2556,14 +2583,14 @@
         <v>53</v>
       </c>
       <c r="H42" s="13"/>
-      <c r="I42" s="77"/>
+      <c r="I42" s="99"/>
     </row>
     <row r="43" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="58"/>
-      <c r="B43" s="78"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
+      <c r="A43" s="86"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="62"/>
+      <c r="E43" s="62"/>
       <c r="F43" s="12" t="s">
         <v>54</v>
       </c>
@@ -2571,14 +2598,14 @@
         <v>55</v>
       </c>
       <c r="H43" s="13"/>
-      <c r="I43" s="77"/>
+      <c r="I43" s="99"/>
     </row>
     <row r="44" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="58"/>
-      <c r="B44" s="78"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
+      <c r="A44" s="86"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="62"/>
+      <c r="E44" s="62"/>
       <c r="F44" s="12" t="s">
         <v>56</v>
       </c>
@@ -2586,14 +2613,14 @@
         <v>57</v>
       </c>
       <c r="H44" s="13"/>
-      <c r="I44" s="77"/>
+      <c r="I44" s="99"/>
     </row>
     <row r="45" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="58"/>
-      <c r="B45" s="78"/>
-      <c r="C45" s="60"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
+      <c r="A45" s="86"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="62"/>
       <c r="F45" s="12" t="s">
         <v>86</v>
       </c>
@@ -2601,14 +2628,14 @@
         <v>58</v>
       </c>
       <c r="H45" s="13"/>
-      <c r="I45" s="77"/>
+      <c r="I45" s="99"/>
     </row>
     <row r="46" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="58"/>
-      <c r="B46" s="78"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
+      <c r="A46" s="86"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+      <c r="E46" s="62"/>
       <c r="F46" s="12" t="s">
         <v>59</v>
       </c>
@@ -2616,14 +2643,14 @@
         <v>60</v>
       </c>
       <c r="H46" s="13"/>
-      <c r="I46" s="77"/>
+      <c r="I46" s="99"/>
     </row>
     <row r="47" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="58"/>
-      <c r="B47" s="78"/>
-      <c r="C47" s="60"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
+      <c r="A47" s="86"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="62"/>
       <c r="F47" s="14" t="s">
         <v>61</v>
       </c>
@@ -2631,22 +2658,22 @@
         <v>62</v>
       </c>
       <c r="H47" s="15"/>
-      <c r="I47" s="77"/>
+      <c r="I47" s="99"/>
     </row>
     <row r="48" spans="1:11" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="58">
+      <c r="A48" s="86">
         <v>11</v>
       </c>
-      <c r="B48" s="78" t="s">
+      <c r="B48" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="60" t="s">
+      <c r="C48" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="60" t="s">
+      <c r="D48" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E48" s="60" t="s">
+      <c r="E48" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F48" s="10" t="s">
@@ -2656,18 +2683,18 @@
         <v>49</v>
       </c>
       <c r="H48" s="11"/>
-      <c r="I48" s="77" t="s">
+      <c r="I48" s="99" t="s">
         <v>12</v>
       </c>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
     </row>
     <row r="49" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="58"/>
-      <c r="B49" s="78"/>
-      <c r="C49" s="60"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
+      <c r="A49" s="86"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+      <c r="E49" s="62"/>
       <c r="F49" s="12" t="s">
         <v>50</v>
       </c>
@@ -2675,16 +2702,16 @@
         <v>51</v>
       </c>
       <c r="H49" s="13"/>
-      <c r="I49" s="77"/>
+      <c r="I49" s="99"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
     </row>
     <row r="50" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="58"/>
-      <c r="B50" s="78"/>
-      <c r="C50" s="60"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
+      <c r="A50" s="86"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+      <c r="E50" s="62"/>
       <c r="F50" s="12" t="s">
         <v>65</v>
       </c>
@@ -2692,16 +2719,16 @@
         <v>53</v>
       </c>
       <c r="H50" s="13"/>
-      <c r="I50" s="77"/>
+      <c r="I50" s="99"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
     </row>
     <row r="51" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="58"/>
-      <c r="B51" s="78"/>
-      <c r="C51" s="60"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
+      <c r="A51" s="86"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+      <c r="E51" s="62"/>
       <c r="F51" s="12" t="s">
         <v>54</v>
       </c>
@@ -2709,16 +2736,16 @@
         <v>55</v>
       </c>
       <c r="H51" s="13"/>
-      <c r="I51" s="77"/>
+      <c r="I51" s="99"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
     </row>
     <row r="52" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A52" s="58"/>
-      <c r="B52" s="78"/>
-      <c r="C52" s="60"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
+      <c r="A52" s="86"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+      <c r="E52" s="62"/>
       <c r="F52" s="12" t="s">
         <v>56</v>
       </c>
@@ -2726,16 +2753,16 @@
         <v>57</v>
       </c>
       <c r="H52" s="13"/>
-      <c r="I52" s="77"/>
+      <c r="I52" s="99"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
     </row>
     <row r="53" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A53" s="58"/>
-      <c r="B53" s="78"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
+      <c r="A53" s="86"/>
+      <c r="B53" s="81"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+      <c r="E53" s="62"/>
       <c r="F53" s="12" t="s">
         <v>86</v>
       </c>
@@ -2743,16 +2770,16 @@
         <v>58</v>
       </c>
       <c r="H53" s="13"/>
-      <c r="I53" s="77"/>
+      <c r="I53" s="99"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
     </row>
     <row r="54" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="58"/>
-      <c r="B54" s="78"/>
-      <c r="C54" s="60"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="60"/>
+      <c r="A54" s="86"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
+      <c r="E54" s="62"/>
       <c r="F54" s="12" t="s">
         <v>59</v>
       </c>
@@ -2760,16 +2787,16 @@
         <v>60</v>
       </c>
       <c r="H54" s="13"/>
-      <c r="I54" s="77"/>
+      <c r="I54" s="99"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
     </row>
     <row r="55" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="58"/>
-      <c r="B55" s="78"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="60"/>
+      <c r="A55" s="86"/>
+      <c r="B55" s="81"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
+      <c r="E55" s="62"/>
       <c r="F55" s="14" t="s">
         <v>61</v>
       </c>
@@ -2777,24 +2804,24 @@
         <v>62</v>
       </c>
       <c r="H55" s="15"/>
-      <c r="I55" s="77"/>
+      <c r="I55" s="99"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
     </row>
     <row r="56" spans="1:11" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="58">
+      <c r="A56" s="86">
         <v>12</v>
       </c>
-      <c r="B56" s="78" t="s">
+      <c r="B56" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="60" t="s">
+      <c r="C56" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="D56" s="60" t="s">
+      <c r="D56" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="60" t="s">
+      <c r="E56" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F56" s="10" t="s">
@@ -2804,18 +2831,18 @@
         <v>49</v>
       </c>
       <c r="H56" s="11"/>
-      <c r="I56" s="77" t="s">
+      <c r="I56" s="99" t="s">
         <v>12</v>
       </c>
       <c r="J56" s="17"/>
       <c r="K56" s="17"/>
     </row>
     <row r="57" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A57" s="58"/>
-      <c r="B57" s="78"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="60"/>
+      <c r="A57" s="86"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
       <c r="F57" s="12" t="s">
         <v>68</v>
       </c>
@@ -2823,16 +2850,16 @@
         <v>69</v>
       </c>
       <c r="H57" s="13"/>
-      <c r="I57" s="77"/>
+      <c r="I57" s="99"/>
       <c r="J57" s="17"/>
       <c r="K57" s="17"/>
     </row>
     <row r="58" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="58"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="60"/>
-      <c r="D58" s="60"/>
-      <c r="E58" s="60"/>
+      <c r="A58" s="86"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+      <c r="E58" s="62"/>
       <c r="F58" s="12" t="s">
         <v>87</v>
       </c>
@@ -2840,16 +2867,16 @@
         <v>88</v>
       </c>
       <c r="H58" s="13"/>
-      <c r="I58" s="77"/>
+      <c r="I58" s="99"/>
       <c r="J58" s="17"/>
       <c r="K58" s="17"/>
     </row>
     <row r="59" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="58"/>
-      <c r="B59" s="78"/>
-      <c r="C59" s="60"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="60"/>
+      <c r="A59" s="86"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+      <c r="E59" s="62"/>
       <c r="F59" s="14" t="s">
         <v>70</v>
       </c>
@@ -2857,24 +2884,24 @@
         <v>71</v>
       </c>
       <c r="H59" s="15"/>
-      <c r="I59" s="77"/>
+      <c r="I59" s="99"/>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
     </row>
     <row r="60" spans="1:11" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="58">
+      <c r="A60" s="86">
         <v>13</v>
       </c>
-      <c r="B60" s="78" t="s">
+      <c r="B60" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="C60" s="60" t="s">
+      <c r="C60" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="D60" s="60" t="s">
+      <c r="D60" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="60" t="s">
+      <c r="E60" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F60" s="10" t="s">
@@ -2884,18 +2911,18 @@
         <v>49</v>
       </c>
       <c r="H60" s="11"/>
-      <c r="I60" s="69" t="s">
+      <c r="I60" s="101" t="s">
         <v>12</v>
       </c>
       <c r="J60" s="17"/>
       <c r="K60" s="17"/>
     </row>
     <row r="61" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A61" s="59"/>
-      <c r="B61" s="105"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
+      <c r="A61" s="87"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="63"/>
+      <c r="D61" s="63"/>
+      <c r="E61" s="63"/>
       <c r="F61" s="12" t="s">
         <v>68</v>
       </c>
@@ -2903,16 +2930,16 @@
         <v>69</v>
       </c>
       <c r="H61" s="13"/>
-      <c r="I61" s="70"/>
+      <c r="I61" s="102"/>
       <c r="J61" s="17"/>
       <c r="K61" s="17"/>
     </row>
     <row r="62" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A62" s="59"/>
-      <c r="B62" s="105"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="61"/>
-      <c r="E62" s="61"/>
+      <c r="A62" s="87"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="63"/>
+      <c r="D62" s="63"/>
+      <c r="E62" s="63"/>
       <c r="F62" s="12" t="s">
         <v>143</v>
       </c>
@@ -2920,16 +2947,16 @@
         <v>146</v>
       </c>
       <c r="H62" s="13"/>
-      <c r="I62" s="70"/>
+      <c r="I62" s="102"/>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
     </row>
     <row r="63" spans="1:11" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="59"/>
-      <c r="B63" s="105"/>
-      <c r="C63" s="61"/>
-      <c r="D63" s="61"/>
-      <c r="E63" s="61"/>
+      <c r="A63" s="87"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
       <c r="F63" s="12" t="s">
         <v>144</v>
       </c>
@@ -2937,16 +2964,16 @@
         <v>147</v>
       </c>
       <c r="H63" s="13"/>
-      <c r="I63" s="70"/>
+      <c r="I63" s="102"/>
       <c r="J63" s="17"/>
       <c r="K63" s="17"/>
     </row>
     <row r="64" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="59"/>
-      <c r="B64" s="105"/>
-      <c r="C64" s="61"/>
-      <c r="D64" s="61"/>
-      <c r="E64" s="61"/>
+      <c r="A64" s="87"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
       <c r="F64" s="14" t="s">
         <v>145</v>
       </c>
@@ -2954,24 +2981,24 @@
         <v>148</v>
       </c>
       <c r="H64" s="15"/>
-      <c r="I64" s="70"/>
+      <c r="I64" s="102"/>
       <c r="J64" s="17"/>
       <c r="K64" s="17"/>
     </row>
     <row r="65" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="58">
+      <c r="A65" s="86">
         <v>14</v>
       </c>
-      <c r="B65" s="78" t="s">
+      <c r="B65" s="81" t="s">
         <v>156</v>
       </c>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="D65" s="60" t="s">
+      <c r="D65" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E65" s="60" t="s">
+      <c r="E65" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F65" s="10" t="s">
@@ -2981,18 +3008,18 @@
         <v>110</v>
       </c>
       <c r="H65" s="11"/>
-      <c r="I65" s="69" t="s">
+      <c r="I65" s="101" t="s">
         <v>163</v>
       </c>
       <c r="J65" s="17"/>
       <c r="K65" s="17"/>
     </row>
     <row r="66" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A66" s="59"/>
-      <c r="B66" s="105"/>
-      <c r="C66" s="61"/>
-      <c r="D66" s="61"/>
-      <c r="E66" s="61"/>
+      <c r="A66" s="87"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="63"/>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
       <c r="F66" s="12" t="s">
         <v>111</v>
       </c>
@@ -3000,16 +3027,16 @@
         <v>168</v>
       </c>
       <c r="H66" s="13"/>
-      <c r="I66" s="70"/>
+      <c r="I66" s="102"/>
       <c r="J66" s="17"/>
       <c r="K66" s="17"/>
     </row>
     <row r="67" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="59"/>
-      <c r="B67" s="105"/>
-      <c r="C67" s="61"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="61"/>
+      <c r="A67" s="87"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
       <c r="F67" s="12" t="s">
         <v>158</v>
       </c>
@@ -3017,16 +3044,16 @@
         <v>113</v>
       </c>
       <c r="H67" s="13"/>
-      <c r="I67" s="70"/>
+      <c r="I67" s="102"/>
       <c r="J67" s="17"/>
       <c r="K67" s="17"/>
     </row>
     <row r="68" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A68" s="59"/>
-      <c r="B68" s="105"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
+      <c r="A68" s="87"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="63"/>
       <c r="F68" s="12" t="s">
         <v>159</v>
       </c>
@@ -3034,16 +3061,16 @@
         <v>161</v>
       </c>
       <c r="H68" s="13"/>
-      <c r="I68" s="70"/>
+      <c r="I68" s="102"/>
       <c r="J68" s="17"/>
       <c r="K68" s="17"/>
     </row>
     <row r="69" spans="1:11" ht="64.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="76"/>
-      <c r="B69" s="109"/>
-      <c r="C69" s="68"/>
-      <c r="D69" s="68"/>
-      <c r="E69" s="68"/>
+      <c r="A69" s="103"/>
+      <c r="B69" s="89"/>
+      <c r="C69" s="64"/>
+      <c r="D69" s="64"/>
+      <c r="E69" s="64"/>
       <c r="F69" s="18" t="s">
         <v>160</v>
       </c>
@@ -3051,24 +3078,24 @@
         <v>162</v>
       </c>
       <c r="H69" s="19"/>
-      <c r="I69" s="71"/>
+      <c r="I69" s="104"/>
       <c r="J69" s="17"/>
       <c r="K69" s="17"/>
     </row>
     <row r="70" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="58">
+      <c r="A70" s="86">
         <v>15</v>
       </c>
-      <c r="B70" s="78" t="s">
+      <c r="B70" s="81" t="s">
         <v>164</v>
       </c>
-      <c r="C70" s="60" t="s">
+      <c r="C70" s="62" t="s">
         <v>165</v>
       </c>
-      <c r="D70" s="60" t="s">
+      <c r="D70" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="60" t="s">
+      <c r="E70" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F70" s="10" t="s">
@@ -3078,18 +3105,18 @@
         <v>110</v>
       </c>
       <c r="H70" s="11"/>
-      <c r="I70" s="69" t="s">
+      <c r="I70" s="101" t="s">
         <v>12</v>
       </c>
       <c r="J70" s="17"/>
       <c r="K70" s="17"/>
     </row>
     <row r="71" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A71" s="59"/>
-      <c r="B71" s="105"/>
-      <c r="C71" s="61"/>
-      <c r="D71" s="61"/>
-      <c r="E71" s="61"/>
+      <c r="A71" s="87"/>
+      <c r="B71" s="61"/>
+      <c r="C71" s="63"/>
+      <c r="D71" s="63"/>
+      <c r="E71" s="63"/>
       <c r="F71" s="21" t="s">
         <v>111</v>
       </c>
@@ -3097,16 +3124,16 @@
         <v>168</v>
       </c>
       <c r="H71" s="22"/>
-      <c r="I71" s="70"/>
+      <c r="I71" s="102"/>
       <c r="J71" s="17"/>
       <c r="K71" s="17"/>
     </row>
     <row r="72" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A72" s="59"/>
-      <c r="B72" s="105"/>
-      <c r="C72" s="61"/>
-      <c r="D72" s="61"/>
-      <c r="E72" s="61"/>
+      <c r="A72" s="87"/>
+      <c r="B72" s="61"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="63"/>
       <c r="F72" s="21" t="s">
         <v>158</v>
       </c>
@@ -3114,16 +3141,16 @@
         <v>113</v>
       </c>
       <c r="H72" s="22"/>
-      <c r="I72" s="70"/>
+      <c r="I72" s="102"/>
       <c r="J72" s="17"/>
       <c r="K72" s="17"/>
     </row>
     <row r="73" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="59"/>
-      <c r="B73" s="105"/>
-      <c r="C73" s="61"/>
-      <c r="D73" s="61"/>
-      <c r="E73" s="61"/>
+      <c r="A73" s="87"/>
+      <c r="B73" s="61"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
       <c r="F73" s="21" t="s">
         <v>159</v>
       </c>
@@ -3131,16 +3158,16 @@
         <v>161</v>
       </c>
       <c r="H73" s="22"/>
-      <c r="I73" s="70"/>
+      <c r="I73" s="102"/>
       <c r="J73" s="17"/>
       <c r="K73" s="17"/>
     </row>
     <row r="74" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="76"/>
-      <c r="B74" s="109"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="68"/>
-      <c r="E74" s="68"/>
+      <c r="A74" s="103"/>
+      <c r="B74" s="89"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="64"/>
       <c r="F74" s="34" t="s">
         <v>166</v>
       </c>
@@ -3148,24 +3175,24 @@
         <v>167</v>
       </c>
       <c r="H74" s="35"/>
-      <c r="I74" s="71"/>
+      <c r="I74" s="104"/>
       <c r="J74" s="17"/>
       <c r="K74" s="17"/>
     </row>
     <row r="75" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="72">
+      <c r="A75" s="100">
         <v>16</v>
       </c>
-      <c r="B75" s="78" t="s">
+      <c r="B75" s="81" t="s">
         <v>169</v>
       </c>
-      <c r="C75" s="60" t="s">
+      <c r="C75" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="D75" s="60" t="s">
+      <c r="D75" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E75" s="60" t="s">
+      <c r="E75" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F75" s="21" t="s">
@@ -3175,18 +3202,18 @@
         <v>110</v>
       </c>
       <c r="H75" s="22"/>
-      <c r="I75" s="60" t="s">
+      <c r="I75" s="62" t="s">
         <v>163</v>
       </c>
       <c r="J75" s="17"/>
       <c r="K75" s="17"/>
     </row>
     <row r="76" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="73"/>
-      <c r="B76" s="105"/>
-      <c r="C76" s="61"/>
-      <c r="D76" s="61"/>
-      <c r="E76" s="61"/>
+      <c r="A76" s="107"/>
+      <c r="B76" s="61"/>
+      <c r="C76" s="63"/>
+      <c r="D76" s="63"/>
+      <c r="E76" s="63"/>
       <c r="F76" s="12" t="s">
         <v>111</v>
       </c>
@@ -3194,16 +3221,16 @@
         <v>168</v>
       </c>
       <c r="H76" s="13"/>
-      <c r="I76" s="61"/>
+      <c r="I76" s="63"/>
       <c r="J76" s="17"/>
       <c r="K76" s="17"/>
     </row>
     <row r="77" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="74"/>
-      <c r="B77" s="110"/>
-      <c r="C77" s="75"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
+      <c r="A77" s="108"/>
+      <c r="B77" s="109"/>
+      <c r="C77" s="110"/>
+      <c r="D77" s="110"/>
+      <c r="E77" s="110"/>
       <c r="F77" s="12" t="s">
         <v>171</v>
       </c>
@@ -3211,24 +3238,24 @@
         <v>172</v>
       </c>
       <c r="H77" s="13"/>
-      <c r="I77" s="75"/>
+      <c r="I77" s="110"/>
       <c r="J77" s="17"/>
       <c r="K77" s="17"/>
     </row>
     <row r="78" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="58">
+      <c r="A78" s="86">
         <v>17</v>
       </c>
-      <c r="B78" s="78" t="s">
+      <c r="B78" s="81" t="s">
         <v>149</v>
       </c>
-      <c r="C78" s="60" t="s">
+      <c r="C78" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="D78" s="60" t="s">
+      <c r="D78" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E78" s="60" t="s">
+      <c r="E78" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F78" s="10" t="s">
@@ -3243,11 +3270,11 @@
       <c r="K78" s="17"/>
     </row>
     <row r="79" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A79" s="59"/>
-      <c r="B79" s="105"/>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
-      <c r="E79" s="61"/>
+      <c r="A79" s="87"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="63"/>
+      <c r="D79" s="63"/>
+      <c r="E79" s="63"/>
       <c r="F79" s="12" t="s">
         <v>102</v>
       </c>
@@ -3260,11 +3287,11 @@
       <c r="K79" s="17"/>
     </row>
     <row r="80" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A80" s="59"/>
-      <c r="B80" s="105"/>
-      <c r="C80" s="61"/>
-      <c r="D80" s="61"/>
-      <c r="E80" s="61"/>
+      <c r="A80" s="87"/>
+      <c r="B80" s="61"/>
+      <c r="C80" s="63"/>
+      <c r="D80" s="63"/>
+      <c r="E80" s="63"/>
       <c r="F80" s="12" t="s">
         <v>103</v>
       </c>
@@ -3277,11 +3304,11 @@
       <c r="K80" s="17"/>
     </row>
     <row r="81" spans="1:11" ht="40.200000000000003" x14ac:dyDescent="0.3">
-      <c r="A81" s="59"/>
-      <c r="B81" s="105"/>
-      <c r="C81" s="61"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="61"/>
+      <c r="A81" s="87"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="63"/>
+      <c r="D81" s="63"/>
+      <c r="E81" s="63"/>
       <c r="F81" s="29" t="s">
         <v>151</v>
       </c>
@@ -3294,11 +3321,11 @@
       <c r="K81" s="17"/>
     </row>
     <row r="82" spans="1:11" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="76"/>
-      <c r="B82" s="109"/>
-      <c r="C82" s="68"/>
-      <c r="D82" s="68"/>
-      <c r="E82" s="68"/>
+      <c r="A82" s="103"/>
+      <c r="B82" s="89"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
       <c r="F82" s="31" t="s">
         <v>152</v>
       </c>
@@ -3311,25 +3338,25 @@
       <c r="K82" s="17"/>
     </row>
     <row r="83" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="59">
+      <c r="A83" s="87">
         <v>18</v>
       </c>
-      <c r="B83" s="105" t="s">
+      <c r="B83" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C83" s="61" t="s">
+      <c r="C83" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="D83" s="61" t="s">
+      <c r="D83" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="E83" s="61" t="s">
+      <c r="E83" s="63" t="s">
         <v>90</v>
       </c>
       <c r="F83" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="G83" s="61" t="s">
+      <c r="G83" s="63" t="s">
         <v>106</v>
       </c>
       <c r="H83" s="22"/>
@@ -3338,139 +3365,139 @@
       <c r="K83" s="17"/>
     </row>
     <row r="84" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A84" s="59"/>
-      <c r="B84" s="105"/>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="61"/>
+      <c r="A84" s="87"/>
+      <c r="B84" s="61"/>
+      <c r="C84" s="63"/>
+      <c r="D84" s="63"/>
+      <c r="E84" s="63"/>
       <c r="F84" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="G84" s="61"/>
+      <c r="G84" s="63"/>
       <c r="H84" s="13"/>
       <c r="I84" s="23"/>
       <c r="J84" s="17"/>
       <c r="K84" s="17"/>
     </row>
     <row r="85" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="59"/>
-      <c r="B85" s="105"/>
-      <c r="C85" s="61"/>
-      <c r="D85" s="61"/>
-      <c r="E85" s="61"/>
+      <c r="A85" s="87"/>
+      <c r="B85" s="61"/>
+      <c r="C85" s="63"/>
+      <c r="D85" s="63"/>
+      <c r="E85" s="63"/>
       <c r="F85" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G85" s="61"/>
+      <c r="G85" s="63"/>
       <c r="H85" s="13"/>
       <c r="I85" s="23"/>
       <c r="J85" s="17"/>
       <c r="K85" s="17"/>
     </row>
     <row r="86" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A86" s="59"/>
-      <c r="B86" s="105"/>
-      <c r="C86" s="61"/>
-      <c r="D86" s="61"/>
-      <c r="E86" s="61"/>
+      <c r="A86" s="87"/>
+      <c r="B86" s="61"/>
+      <c r="C86" s="63"/>
+      <c r="D86" s="63"/>
+      <c r="E86" s="63"/>
       <c r="F86" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="G86" s="61"/>
+      <c r="G86" s="63"/>
       <c r="H86" s="13"/>
       <c r="I86" s="23"/>
       <c r="J86" s="17"/>
       <c r="K86" s="17"/>
     </row>
     <row r="87" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A87" s="59"/>
-      <c r="B87" s="105"/>
-      <c r="C87" s="61"/>
-      <c r="D87" s="61"/>
-      <c r="E87" s="61"/>
+      <c r="A87" s="87"/>
+      <c r="B87" s="61"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="63"/>
       <c r="F87" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G87" s="61"/>
+      <c r="G87" s="63"/>
       <c r="H87" s="13"/>
       <c r="I87" s="23"/>
       <c r="J87" s="17"/>
       <c r="K87" s="17"/>
     </row>
     <row r="88" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A88" s="59"/>
-      <c r="B88" s="105"/>
-      <c r="C88" s="61"/>
-      <c r="D88" s="61"/>
-      <c r="E88" s="61"/>
+      <c r="A88" s="87"/>
+      <c r="B88" s="61"/>
+      <c r="C88" s="63"/>
+      <c r="D88" s="63"/>
+      <c r="E88" s="63"/>
       <c r="F88" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G88" s="61"/>
+      <c r="G88" s="63"/>
       <c r="H88" s="13"/>
       <c r="I88" s="23"/>
       <c r="J88" s="17"/>
       <c r="K88" s="17"/>
     </row>
     <row r="89" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="59"/>
-      <c r="B89" s="105"/>
-      <c r="C89" s="61"/>
-      <c r="D89" s="61"/>
-      <c r="E89" s="61"/>
+      <c r="A89" s="87"/>
+      <c r="B89" s="61"/>
+      <c r="C89" s="63"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="63"/>
       <c r="F89" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G89" s="61"/>
+      <c r="G89" s="63"/>
       <c r="H89" s="13"/>
       <c r="I89" s="23"/>
       <c r="J89" s="17"/>
       <c r="K89" s="17"/>
     </row>
     <row r="90" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="59"/>
-      <c r="B90" s="105"/>
-      <c r="C90" s="61"/>
-      <c r="D90" s="61"/>
-      <c r="E90" s="61"/>
+      <c r="A90" s="87"/>
+      <c r="B90" s="61"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="63"/>
       <c r="F90" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G90" s="61"/>
+      <c r="G90" s="63"/>
       <c r="H90" s="13"/>
       <c r="I90" s="23"/>
       <c r="J90" s="17"/>
       <c r="K90" s="17"/>
     </row>
     <row r="91" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="59"/>
-      <c r="B91" s="105"/>
-      <c r="C91" s="61"/>
-      <c r="D91" s="61"/>
-      <c r="E91" s="61"/>
+      <c r="A91" s="87"/>
+      <c r="B91" s="61"/>
+      <c r="C91" s="63"/>
+      <c r="D91" s="63"/>
+      <c r="E91" s="63"/>
       <c r="F91" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G91" s="61"/>
+      <c r="G91" s="63"/>
       <c r="H91" s="15"/>
       <c r="I91" s="24"/>
       <c r="J91" s="17"/>
       <c r="K91" s="17"/>
     </row>
     <row r="92" spans="1:11" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="58">
+      <c r="A92" s="86">
         <v>19</v>
       </c>
-      <c r="B92" s="78" t="s">
+      <c r="B92" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C92" s="60" t="s">
+      <c r="C92" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="D92" s="60" t="s">
+      <c r="D92" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E92" s="60" t="s">
+      <c r="E92" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F92" s="10" t="s">
@@ -3485,11 +3512,11 @@
       <c r="K92" s="17"/>
     </row>
     <row r="93" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="59"/>
-      <c r="B93" s="105"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61"/>
-      <c r="E93" s="61"/>
+      <c r="A93" s="87"/>
+      <c r="B93" s="61"/>
+      <c r="C93" s="63"/>
+      <c r="D93" s="63"/>
+      <c r="E93" s="63"/>
       <c r="F93" s="12" t="s">
         <v>111</v>
       </c>
@@ -3502,11 +3529,11 @@
       <c r="K93" s="17"/>
     </row>
     <row r="94" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="59"/>
-      <c r="B94" s="105"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-      <c r="E94" s="61"/>
+      <c r="A94" s="87"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="63"/>
+      <c r="E94" s="63"/>
       <c r="F94" s="12" t="s">
         <v>103</v>
       </c>
@@ -3519,11 +3546,11 @@
       <c r="K94" s="17"/>
     </row>
     <row r="95" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A95" s="59"/>
-      <c r="B95" s="105"/>
-      <c r="C95" s="61"/>
-      <c r="D95" s="61"/>
-      <c r="E95" s="61"/>
+      <c r="A95" s="87"/>
+      <c r="B95" s="61"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="63"/>
+      <c r="E95" s="63"/>
       <c r="F95" s="12" t="s">
         <v>104</v>
       </c>
@@ -3536,11 +3563,11 @@
       <c r="K95" s="17"/>
     </row>
     <row r="96" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A96" s="59"/>
-      <c r="B96" s="105"/>
-      <c r="C96" s="61"/>
-      <c r="D96" s="61"/>
-      <c r="E96" s="61"/>
+      <c r="A96" s="87"/>
+      <c r="B96" s="61"/>
+      <c r="C96" s="63"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="63"/>
       <c r="F96" s="12" t="s">
         <v>108</v>
       </c>
@@ -3553,11 +3580,11 @@
       <c r="K96" s="17"/>
     </row>
     <row r="97" spans="1:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="59"/>
-      <c r="B97" s="105"/>
-      <c r="C97" s="61"/>
-      <c r="D97" s="61"/>
-      <c r="E97" s="61"/>
+      <c r="A97" s="87"/>
+      <c r="B97" s="61"/>
+      <c r="C97" s="63"/>
+      <c r="D97" s="63"/>
+      <c r="E97" s="63"/>
       <c r="F97" s="14" t="s">
         <v>109</v>
       </c>
@@ -3570,19 +3597,19 @@
       <c r="K97" s="17"/>
     </row>
     <row r="98" spans="1:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="58">
+      <c r="A98" s="86">
         <v>20</v>
       </c>
-      <c r="B98" s="78" t="s">
+      <c r="B98" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="C98" s="60" t="s">
+      <c r="C98" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="D98" s="60" t="s">
+      <c r="D98" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="E98" s="60" t="s">
+      <c r="E98" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F98" s="10" t="s">
@@ -3597,11 +3624,11 @@
       <c r="K98" s="17"/>
     </row>
     <row r="99" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="59"/>
-      <c r="B99" s="105"/>
-      <c r="C99" s="61"/>
-      <c r="D99" s="61"/>
-      <c r="E99" s="61"/>
+      <c r="A99" s="87"/>
+      <c r="B99" s="61"/>
+      <c r="C99" s="63"/>
+      <c r="D99" s="63"/>
+      <c r="E99" s="63"/>
       <c r="F99" s="12" t="s">
         <v>111</v>
       </c>
@@ -3614,11 +3641,11 @@
       <c r="K99" s="17"/>
     </row>
     <row r="100" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="59"/>
-      <c r="B100" s="105"/>
-      <c r="C100" s="61"/>
-      <c r="D100" s="61"/>
-      <c r="E100" s="61"/>
+      <c r="A100" s="87"/>
+      <c r="B100" s="61"/>
+      <c r="C100" s="63"/>
+      <c r="D100" s="63"/>
+      <c r="E100" s="63"/>
       <c r="F100" s="12" t="s">
         <v>103</v>
       </c>
@@ -3631,11 +3658,11 @@
       <c r="K100" s="17"/>
     </row>
     <row r="101" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="59"/>
-      <c r="B101" s="105"/>
-      <c r="C101" s="61"/>
-      <c r="D101" s="61"/>
-      <c r="E101" s="61"/>
+      <c r="A101" s="87"/>
+      <c r="B101" s="61"/>
+      <c r="C101" s="63"/>
+      <c r="D101" s="63"/>
+      <c r="E101" s="63"/>
       <c r="F101" s="12" t="s">
         <v>104</v>
       </c>
@@ -3648,11 +3675,11 @@
       <c r="K101" s="17"/>
     </row>
     <row r="102" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="59"/>
-      <c r="B102" s="105"/>
-      <c r="C102" s="61"/>
-      <c r="D102" s="61"/>
-      <c r="E102" s="61"/>
+      <c r="A102" s="87"/>
+      <c r="B102" s="61"/>
+      <c r="C102" s="63"/>
+      <c r="D102" s="63"/>
+      <c r="E102" s="63"/>
       <c r="F102" s="14" t="s">
         <v>120</v>
       </c>
@@ -3665,19 +3692,19 @@
       <c r="K102" s="17"/>
     </row>
     <row r="103" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="58">
+      <c r="A103" s="86">
         <v>21</v>
       </c>
-      <c r="B103" s="78" t="s">
+      <c r="B103" s="81" t="s">
         <v>122</v>
       </c>
-      <c r="C103" s="60" t="s">
+      <c r="C103" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="D103" s="60" t="s">
+      <c r="D103" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E103" s="60" t="s">
+      <c r="E103" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F103" s="10" t="s">
@@ -3692,11 +3719,11 @@
       <c r="K103" s="17"/>
     </row>
     <row r="104" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A104" s="59"/>
-      <c r="B104" s="105"/>
-      <c r="C104" s="61"/>
-      <c r="D104" s="61"/>
-      <c r="E104" s="61"/>
+      <c r="A104" s="87"/>
+      <c r="B104" s="61"/>
+      <c r="C104" s="63"/>
+      <c r="D104" s="63"/>
+      <c r="E104" s="63"/>
       <c r="F104" s="12" t="s">
         <v>111</v>
       </c>
@@ -3709,11 +3736,11 @@
       <c r="K104" s="17"/>
     </row>
     <row r="105" spans="1:11" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A105" s="59"/>
-      <c r="B105" s="105"/>
-      <c r="C105" s="61"/>
-      <c r="D105" s="61"/>
-      <c r="E105" s="61"/>
+      <c r="A105" s="87"/>
+      <c r="B105" s="61"/>
+      <c r="C105" s="63"/>
+      <c r="D105" s="63"/>
+      <c r="E105" s="63"/>
       <c r="F105" s="12" t="s">
         <v>124</v>
       </c>
@@ -3726,11 +3753,11 @@
       <c r="K105" s="17"/>
     </row>
     <row r="106" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A106" s="59"/>
-      <c r="B106" s="105"/>
-      <c r="C106" s="61"/>
-      <c r="D106" s="61"/>
-      <c r="E106" s="61"/>
+      <c r="A106" s="87"/>
+      <c r="B106" s="61"/>
+      <c r="C106" s="63"/>
+      <c r="D106" s="63"/>
+      <c r="E106" s="63"/>
       <c r="F106" s="12" t="s">
         <v>125</v>
       </c>
@@ -3743,11 +3770,11 @@
       <c r="K106" s="17"/>
     </row>
     <row r="107" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A107" s="59"/>
-      <c r="B107" s="105"/>
-      <c r="C107" s="61"/>
-      <c r="D107" s="61"/>
-      <c r="E107" s="61"/>
+      <c r="A107" s="87"/>
+      <c r="B107" s="61"/>
+      <c r="C107" s="63"/>
+      <c r="D107" s="63"/>
+      <c r="E107" s="63"/>
       <c r="F107" s="12" t="s">
         <v>126</v>
       </c>
@@ -3760,11 +3787,11 @@
       <c r="K107" s="17"/>
     </row>
     <row r="108" spans="1:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="59"/>
-      <c r="B108" s="105"/>
-      <c r="C108" s="61"/>
-      <c r="D108" s="61"/>
-      <c r="E108" s="61"/>
+      <c r="A108" s="87"/>
+      <c r="B108" s="61"/>
+      <c r="C108" s="63"/>
+      <c r="D108" s="63"/>
+      <c r="E108" s="63"/>
       <c r="F108" s="14" t="s">
         <v>127</v>
       </c>
@@ -3777,19 +3804,19 @@
       <c r="K108" s="17"/>
     </row>
     <row r="109" spans="1:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="58">
+      <c r="A109" s="86">
         <v>22</v>
       </c>
-      <c r="B109" s="78" t="s">
+      <c r="B109" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="C109" s="60" t="s">
+      <c r="C109" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="D109" s="60" t="s">
+      <c r="D109" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="E109" s="60" t="s">
+      <c r="E109" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F109" s="10" t="s">
@@ -3804,11 +3831,11 @@
       <c r="K109" s="17"/>
     </row>
     <row r="110" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A110" s="59"/>
-      <c r="B110" s="105"/>
-      <c r="C110" s="61"/>
-      <c r="D110" s="61"/>
-      <c r="E110" s="61"/>
+      <c r="A110" s="87"/>
+      <c r="B110" s="61"/>
+      <c r="C110" s="63"/>
+      <c r="D110" s="63"/>
+      <c r="E110" s="63"/>
       <c r="F110" s="12" t="s">
         <v>135</v>
       </c>
@@ -3821,11 +3848,11 @@
       <c r="K110" s="17"/>
     </row>
     <row r="111" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="76"/>
-      <c r="B111" s="109"/>
-      <c r="C111" s="68"/>
-      <c r="D111" s="68"/>
-      <c r="E111" s="68"/>
+      <c r="A111" s="103"/>
+      <c r="B111" s="89"/>
+      <c r="C111" s="64"/>
+      <c r="D111" s="64"/>
+      <c r="E111" s="64"/>
       <c r="F111" s="18" t="s">
         <v>136</v>
       </c>
@@ -3841,16 +3868,16 @@
       <c r="A112" s="84">
         <v>23</v>
       </c>
-      <c r="B112" s="104" t="s">
+      <c r="B112" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="C112" s="60" t="s">
+      <c r="C112" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="D112" s="60" t="s">
+      <c r="D112" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="E112" s="60" t="s">
+      <c r="E112" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F112" s="10" t="s">
@@ -3860,7 +3887,7 @@
         <v>75</v>
       </c>
       <c r="H112" s="11"/>
-      <c r="I112" s="77" t="s">
+      <c r="I112" s="99" t="s">
         <v>12</v>
       </c>
       <c r="J112" s="17"/>
@@ -3868,10 +3895,10 @@
     </row>
     <row r="113" spans="1:11" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A113" s="84"/>
-      <c r="B113" s="104"/>
-      <c r="C113" s="60"/>
-      <c r="D113" s="60"/>
-      <c r="E113" s="60"/>
+      <c r="B113" s="85"/>
+      <c r="C113" s="62"/>
+      <c r="D113" s="62"/>
+      <c r="E113" s="62"/>
       <c r="F113" s="12" t="s">
         <v>76</v>
       </c>
@@ -3879,7 +3906,7 @@
         <v>77</v>
       </c>
       <c r="H113" s="13"/>
-      <c r="I113" s="77"/>
+      <c r="I113" s="99"/>
       <c r="J113" s="17"/>
       <c r="K113" s="17"/>
     </row>
@@ -3887,16 +3914,16 @@
       <c r="A114" s="84">
         <v>24</v>
       </c>
-      <c r="B114" s="85" t="s">
+      <c r="B114" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="C114" s="86" t="s">
+      <c r="C114" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="D114" s="86" t="s">
+      <c r="D114" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="E114" s="86" t="s">
+      <c r="E114" s="98" t="s">
         <v>90</v>
       </c>
       <c r="F114" s="10" t="s">
@@ -3906,17 +3933,17 @@
         <v>81</v>
       </c>
       <c r="H114" s="11"/>
-      <c r="I114" s="79" t="s">
+      <c r="I114" s="92" t="s">
         <v>12</v>
       </c>
       <c r="J114" s="17"/>
     </row>
     <row r="115" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A115" s="84"/>
-      <c r="B115" s="85"/>
-      <c r="C115" s="86"/>
-      <c r="D115" s="86"/>
-      <c r="E115" s="86"/>
+      <c r="B115" s="97"/>
+      <c r="C115" s="98"/>
+      <c r="D115" s="98"/>
+      <c r="E115" s="98"/>
       <c r="F115" s="12" t="s">
         <v>82</v>
       </c>
@@ -3924,23 +3951,23 @@
         <v>83</v>
       </c>
       <c r="H115" s="13"/>
-      <c r="I115" s="79"/>
+      <c r="I115" s="92"/>
       <c r="J115" s="17"/>
     </row>
     <row r="116" spans="1:11" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="80">
+      <c r="A116" s="93">
         <v>25</v>
       </c>
-      <c r="B116" s="81" t="s">
+      <c r="B116" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="C116" s="82" t="s">
+      <c r="C116" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="D116" s="82" t="s">
+      <c r="D116" s="95" t="s">
         <v>36</v>
       </c>
-      <c r="E116" s="82" t="s">
+      <c r="E116" s="95" t="s">
         <v>90</v>
       </c>
       <c r="F116" s="10" t="s">
@@ -3950,16 +3977,16 @@
         <v>81</v>
       </c>
       <c r="H116" s="11"/>
-      <c r="I116" s="83" t="s">
+      <c r="I116" s="96" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="80"/>
-      <c r="B117" s="81"/>
-      <c r="C117" s="82"/>
-      <c r="D117" s="82"/>
-      <c r="E117" s="82"/>
+      <c r="A117" s="93"/>
+      <c r="B117" s="94"/>
+      <c r="C117" s="95"/>
+      <c r="D117" s="95"/>
+      <c r="E117" s="95"/>
       <c r="F117" s="12" t="s">
         <v>85</v>
       </c>
@@ -3967,22 +3994,22 @@
         <v>83</v>
       </c>
       <c r="H117" s="13"/>
-      <c r="I117" s="83"/>
+      <c r="I117" s="96"/>
     </row>
     <row r="118" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A118" s="64">
+      <c r="A118" s="105">
         <v>26</v>
       </c>
-      <c r="B118" s="78" t="s">
+      <c r="B118" s="81" t="s">
         <v>173</v>
       </c>
-      <c r="C118" s="60" t="s">
+      <c r="C118" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="D118" s="66" t="s">
+      <c r="D118" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="E118" s="60" t="s">
+      <c r="E118" s="62" t="s">
         <v>89</v>
       </c>
       <c r="F118" s="10" t="s">
@@ -3992,16 +4019,16 @@
         <v>179</v>
       </c>
       <c r="H118" s="38"/>
-      <c r="I118" s="62" t="s">
+      <c r="I118" s="74" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A119" s="65"/>
-      <c r="B119" s="105"/>
-      <c r="C119" s="61"/>
-      <c r="D119" s="67"/>
-      <c r="E119" s="61"/>
+      <c r="A119" s="106"/>
+      <c r="B119" s="61"/>
+      <c r="C119" s="63"/>
+      <c r="D119" s="72"/>
+      <c r="E119" s="63"/>
       <c r="F119" s="12" t="s">
         <v>176</v>
       </c>
@@ -4009,14 +4036,14 @@
         <v>180</v>
       </c>
       <c r="H119" s="26"/>
-      <c r="I119" s="63"/>
+      <c r="I119" s="75"/>
     </row>
     <row r="120" spans="1:11" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A120" s="65"/>
-      <c r="B120" s="105"/>
-      <c r="C120" s="61"/>
-      <c r="D120" s="67"/>
-      <c r="E120" s="61"/>
+      <c r="A120" s="106"/>
+      <c r="B120" s="61"/>
+      <c r="C120" s="63"/>
+      <c r="D120" s="72"/>
+      <c r="E120" s="63"/>
       <c r="F120" s="12" t="s">
         <v>177</v>
       </c>
@@ -4024,14 +4051,14 @@
         <v>181</v>
       </c>
       <c r="H120" s="26"/>
-      <c r="I120" s="63"/>
+      <c r="I120" s="75"/>
     </row>
     <row r="121" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="65"/>
-      <c r="B121" s="105"/>
-      <c r="C121" s="61"/>
-      <c r="D121" s="67"/>
-      <c r="E121" s="61"/>
+      <c r="A121" s="106"/>
+      <c r="B121" s="61"/>
+      <c r="C121" s="63"/>
+      <c r="D121" s="72"/>
+      <c r="E121" s="63"/>
       <c r="F121" s="14" t="s">
         <v>178</v>
       </c>
@@ -4039,22 +4066,22 @@
         <v>182</v>
       </c>
       <c r="H121" s="41"/>
-      <c r="I121" s="63"/>
+      <c r="I121" s="75"/>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A122" s="99">
+      <c r="A122" s="68">
         <v>27</v>
       </c>
-      <c r="B122" s="106" t="s">
+      <c r="B122" s="65" t="s">
         <v>184</v>
       </c>
-      <c r="C122" s="60" t="s">
+      <c r="C122" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="D122" s="66" t="s">
+      <c r="D122" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="E122" s="60" t="s">
+      <c r="E122" s="62" t="s">
         <v>90</v>
       </c>
       <c r="F122" s="10" t="s">
@@ -4064,16 +4091,16 @@
         <v>188</v>
       </c>
       <c r="H122" s="38"/>
-      <c r="I122" s="62" t="s">
+      <c r="I122" s="74" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:11" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="100"/>
-      <c r="B123" s="107"/>
-      <c r="C123" s="61"/>
-      <c r="D123" s="67"/>
-      <c r="E123" s="61"/>
+      <c r="A123" s="69"/>
+      <c r="B123" s="66"/>
+      <c r="C123" s="63"/>
+      <c r="D123" s="72"/>
+      <c r="E123" s="63"/>
       <c r="F123" s="12" t="s">
         <v>186</v>
       </c>
@@ -4081,14 +4108,14 @@
         <v>208</v>
       </c>
       <c r="H123" s="26"/>
-      <c r="I123" s="63"/>
+      <c r="I123" s="75"/>
     </row>
     <row r="124" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="101"/>
-      <c r="B124" s="108"/>
-      <c r="C124" s="68"/>
-      <c r="D124" s="102"/>
-      <c r="E124" s="68"/>
+      <c r="A124" s="70"/>
+      <c r="B124" s="67"/>
+      <c r="C124" s="64"/>
+      <c r="D124" s="73"/>
+      <c r="E124" s="64"/>
       <c r="F124" s="18" t="s">
         <v>187</v>
       </c>
@@ -4096,7 +4123,7 @@
         <v>189</v>
       </c>
       <c r="H124" s="32"/>
-      <c r="I124" s="103"/>
+      <c r="I124" s="76"/>
     </row>
     <row r="125" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A125" s="42">
@@ -4124,19 +4151,19 @@
       </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126" s="87">
+      <c r="A126" s="82">
         <v>29</v>
       </c>
-      <c r="B126" s="78" t="s">
+      <c r="B126" s="81" t="s">
         <v>195</v>
       </c>
-      <c r="C126" s="90" t="s">
+      <c r="C126" s="77" t="s">
         <v>202</v>
       </c>
-      <c r="D126" s="93" t="s">
+      <c r="D126" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="E126" s="90" t="s">
+      <c r="E126" s="77" t="s">
         <v>90</v>
       </c>
       <c r="F126" s="50" t="s">
@@ -4146,16 +4173,16 @@
         <v>198</v>
       </c>
       <c r="H126" s="38"/>
-      <c r="I126" s="62" t="s">
+      <c r="I126" s="74" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="127" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="88"/>
-      <c r="B127" s="105"/>
-      <c r="C127" s="91"/>
-      <c r="D127" s="94"/>
-      <c r="E127" s="91"/>
+      <c r="A127" s="83"/>
+      <c r="B127" s="61"/>
+      <c r="C127" s="78"/>
+      <c r="D127" s="80"/>
+      <c r="E127" s="78"/>
       <c r="F127" s="48" t="s">
         <v>196</v>
       </c>
@@ -4163,14 +4190,14 @@
         <v>199</v>
       </c>
       <c r="H127" s="26"/>
-      <c r="I127" s="63"/>
+      <c r="I127" s="75"/>
     </row>
     <row r="128" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="88"/>
-      <c r="B128" s="105"/>
-      <c r="C128" s="91"/>
-      <c r="D128" s="94"/>
-      <c r="E128" s="91"/>
+      <c r="A128" s="83"/>
+      <c r="B128" s="61"/>
+      <c r="C128" s="78"/>
+      <c r="D128" s="80"/>
+      <c r="E128" s="78"/>
       <c r="F128" s="52" t="s">
         <v>197</v>
       </c>
@@ -4178,22 +4205,22 @@
         <v>200</v>
       </c>
       <c r="H128" s="41"/>
-      <c r="I128" s="63"/>
+      <c r="I128" s="75"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" s="87">
+      <c r="A129" s="82">
         <v>30</v>
       </c>
-      <c r="B129" s="78" t="s">
+      <c r="B129" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="C129" s="90" t="s">
+      <c r="C129" s="77" t="s">
         <v>203</v>
       </c>
-      <c r="D129" s="93" t="s">
+      <c r="D129" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="E129" s="90" t="s">
+      <c r="E129" s="77" t="s">
         <v>90</v>
       </c>
       <c r="F129" s="56" t="s">
@@ -4203,16 +4230,16 @@
         <v>198</v>
       </c>
       <c r="H129" s="38"/>
-      <c r="I129" s="96" t="s">
+      <c r="I129" s="58" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="88"/>
-      <c r="B130" s="105"/>
-      <c r="C130" s="91"/>
-      <c r="D130" s="94"/>
-      <c r="E130" s="91"/>
+    <row r="130" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="83"/>
+      <c r="B130" s="61"/>
+      <c r="C130" s="78"/>
+      <c r="D130" s="80"/>
+      <c r="E130" s="78"/>
       <c r="F130" s="49" t="s">
         <v>204</v>
       </c>
@@ -4220,14 +4247,14 @@
         <v>206</v>
       </c>
       <c r="H130" s="26"/>
-      <c r="I130" s="97"/>
-    </row>
-    <row r="131" spans="1:9" ht="25.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="89"/>
-      <c r="B131" s="109"/>
-      <c r="C131" s="92"/>
-      <c r="D131" s="95"/>
-      <c r="E131" s="92"/>
+      <c r="I130" s="59"/>
+    </row>
+    <row r="131" spans="1:9" ht="34.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="88"/>
+      <c r="B131" s="89"/>
+      <c r="C131" s="90"/>
+      <c r="D131" s="91"/>
+      <c r="E131" s="90"/>
       <c r="F131" s="51" t="s">
         <v>205</v>
       </c>
@@ -4235,13 +4262,356 @@
         <v>207</v>
       </c>
       <c r="H131" s="32"/>
-      <c r="I131" s="98"/>
-    </row>
-    <row r="133" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="I131" s="60"/>
+    </row>
+    <row r="132" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="86">
+        <v>31</v>
+      </c>
+      <c r="B132" s="81" t="s">
+        <v>209</v>
+      </c>
+      <c r="C132" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="D132" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" s="62" t="s">
+        <v>90</v>
+      </c>
+      <c r="F132" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G132" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H132" s="111"/>
+      <c r="I132" s="99" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="86"/>
+      <c r="B133" s="81"/>
+      <c r="C133" s="62"/>
+      <c r="D133" s="62"/>
+      <c r="E133" s="62"/>
+      <c r="F133" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G133" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H133" s="112"/>
+      <c r="I133" s="99"/>
+    </row>
+    <row r="134" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="86"/>
+      <c r="B134" s="81"/>
+      <c r="C134" s="62"/>
+      <c r="D134" s="62"/>
+      <c r="E134" s="62"/>
+      <c r="F134" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G134" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H134" s="112"/>
+      <c r="I134" s="99"/>
+    </row>
+    <row r="135" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A135" s="86"/>
+      <c r="B135" s="81"/>
+      <c r="C135" s="62"/>
+      <c r="D135" s="62"/>
+      <c r="E135" s="62"/>
+      <c r="F135" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G135" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H135" s="112"/>
+      <c r="I135" s="99"/>
+    </row>
+    <row r="136" spans="1:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="86"/>
+      <c r="B136" s="81"/>
+      <c r="C136" s="62"/>
+      <c r="D136" s="62"/>
+      <c r="E136" s="62"/>
+      <c r="F136" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G136" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H136" s="112"/>
+      <c r="I136" s="99"/>
+    </row>
+    <row r="137" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="93"/>
+      <c r="B137" s="94"/>
+      <c r="C137" s="95"/>
+      <c r="D137" s="95"/>
+      <c r="E137" s="95"/>
+      <c r="F137" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="G137" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="H137" s="113"/>
+      <c r="I137" s="96"/>
+    </row>
+    <row r="138" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="84">
+        <v>32</v>
+      </c>
+      <c r="B138" s="97" t="s">
+        <v>212</v>
+      </c>
+      <c r="C138" s="98" t="s">
+        <v>47</v>
+      </c>
+      <c r="D138" s="98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" s="98" t="s">
+        <v>90</v>
+      </c>
+      <c r="F138" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G138" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H138" s="111"/>
+      <c r="I138" s="92" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="84"/>
+      <c r="B139" s="97"/>
+      <c r="C139" s="98"/>
+      <c r="D139" s="98"/>
+      <c r="E139" s="98"/>
+      <c r="F139" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G139" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H139" s="112"/>
+      <c r="I139" s="92"/>
+    </row>
+    <row r="140" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="84"/>
+      <c r="B140" s="97"/>
+      <c r="C140" s="98"/>
+      <c r="D140" s="98"/>
+      <c r="E140" s="98"/>
+      <c r="F140" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G140" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H140" s="112"/>
+      <c r="I140" s="92"/>
+    </row>
+    <row r="141" spans="1:9" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="84"/>
+      <c r="B141" s="97"/>
+      <c r="C141" s="98"/>
+      <c r="D141" s="98"/>
+      <c r="E141" s="98"/>
+      <c r="F141" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G141" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H141" s="112"/>
+      <c r="I141" s="92"/>
+    </row>
+    <row r="142" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A142" s="84"/>
+      <c r="B142" s="97"/>
+      <c r="C142" s="98"/>
+      <c r="D142" s="98"/>
+      <c r="E142" s="98"/>
+      <c r="F142" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="G142" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="H142" s="112"/>
+      <c r="I142" s="92"/>
+    </row>
   </sheetData>
-  <mergeCells count="169">
+  <mergeCells count="181">
+    <mergeCell ref="I132:I137"/>
+    <mergeCell ref="A138:A142"/>
+    <mergeCell ref="B138:B142"/>
+    <mergeCell ref="C138:C142"/>
+    <mergeCell ref="D138:D142"/>
+    <mergeCell ref="E138:E142"/>
+    <mergeCell ref="I138:I142"/>
+    <mergeCell ref="C98:C102"/>
+    <mergeCell ref="D98:D102"/>
+    <mergeCell ref="E98:E102"/>
+    <mergeCell ref="A83:A91"/>
+    <mergeCell ref="A132:A137"/>
+    <mergeCell ref="B132:B137"/>
+    <mergeCell ref="C132:C137"/>
+    <mergeCell ref="D132:D137"/>
+    <mergeCell ref="E132:E137"/>
+    <mergeCell ref="E118:E121"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="I70:I74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="C75:C77"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="I75:I77"/>
+    <mergeCell ref="A109:A111"/>
+    <mergeCell ref="B109:B111"/>
+    <mergeCell ref="C109:C111"/>
+    <mergeCell ref="D109:D111"/>
+    <mergeCell ref="E109:E111"/>
+    <mergeCell ref="C92:C97"/>
+    <mergeCell ref="D92:D97"/>
+    <mergeCell ref="E92:E97"/>
+    <mergeCell ref="A98:A102"/>
+    <mergeCell ref="B98:B102"/>
+    <mergeCell ref="A103:A108"/>
+    <mergeCell ref="B103:B108"/>
+    <mergeCell ref="C103:C108"/>
+    <mergeCell ref="D103:D108"/>
+    <mergeCell ref="E103:E108"/>
+    <mergeCell ref="I60:I64"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="D78:D82"/>
+    <mergeCell ref="E78:E82"/>
+    <mergeCell ref="A65:A69"/>
+    <mergeCell ref="B65:B69"/>
+    <mergeCell ref="C65:C69"/>
+    <mergeCell ref="D65:D69"/>
+    <mergeCell ref="E65:E69"/>
+    <mergeCell ref="I65:I69"/>
+    <mergeCell ref="A70:A74"/>
+    <mergeCell ref="B70:B74"/>
+    <mergeCell ref="C70:C74"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="C60:C64"/>
+    <mergeCell ref="D60:D64"/>
+    <mergeCell ref="E60:E64"/>
+    <mergeCell ref="I2:I5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="D6:D11"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="I6:I11"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="I20:I23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="D24:D27"/>
+    <mergeCell ref="E24:E27"/>
+    <mergeCell ref="I24:I27"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="E20:E23"/>
+    <mergeCell ref="A56:A59"/>
+    <mergeCell ref="B56:B59"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="D56:D59"/>
+    <mergeCell ref="E56:E59"/>
+    <mergeCell ref="I56:I59"/>
+    <mergeCell ref="A48:A55"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="C32:C35"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="E28:E31"/>
+    <mergeCell ref="I36:I39"/>
+    <mergeCell ref="A40:A47"/>
+    <mergeCell ref="B40:B47"/>
+    <mergeCell ref="C40:C47"/>
+    <mergeCell ref="D40:D47"/>
+    <mergeCell ref="E40:E47"/>
+    <mergeCell ref="I40:I47"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="B48:B55"/>
+    <mergeCell ref="C48:C55"/>
+    <mergeCell ref="D48:D55"/>
+    <mergeCell ref="E48:E55"/>
+    <mergeCell ref="I48:I55"/>
+    <mergeCell ref="B129:B131"/>
+    <mergeCell ref="C129:C131"/>
+    <mergeCell ref="D129:D131"/>
+    <mergeCell ref="E129:E131"/>
+    <mergeCell ref="D112:D113"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="I114:I115"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="D116:D117"/>
+    <mergeCell ref="E116:E117"/>
+    <mergeCell ref="I116:I117"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="D114:D115"/>
+    <mergeCell ref="E114:E115"/>
+    <mergeCell ref="I112:I113"/>
+    <mergeCell ref="I118:I121"/>
+    <mergeCell ref="A118:A121"/>
+    <mergeCell ref="B118:B121"/>
+    <mergeCell ref="C118:C121"/>
+    <mergeCell ref="D118:D121"/>
     <mergeCell ref="I129:I131"/>
     <mergeCell ref="B83:B91"/>
     <mergeCell ref="C122:C124"/>
@@ -4266,151 +4636,6 @@
     <mergeCell ref="D83:D91"/>
     <mergeCell ref="C83:C91"/>
     <mergeCell ref="A129:A131"/>
-    <mergeCell ref="B129:B131"/>
-    <mergeCell ref="C129:C131"/>
-    <mergeCell ref="D129:D131"/>
-    <mergeCell ref="E129:E131"/>
-    <mergeCell ref="D112:D113"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="I114:I115"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="D116:D117"/>
-    <mergeCell ref="E116:E117"/>
-    <mergeCell ref="I116:I117"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="D114:D115"/>
-    <mergeCell ref="E114:E115"/>
-    <mergeCell ref="I112:I113"/>
-    <mergeCell ref="D40:D47"/>
-    <mergeCell ref="E40:E47"/>
-    <mergeCell ref="I40:I47"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="B36:B39"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="E36:E39"/>
-    <mergeCell ref="B48:B55"/>
-    <mergeCell ref="C48:C55"/>
-    <mergeCell ref="D48:D55"/>
-    <mergeCell ref="E48:E55"/>
-    <mergeCell ref="I48:I55"/>
-    <mergeCell ref="A56:A59"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="E56:E59"/>
-    <mergeCell ref="I56:I59"/>
-    <mergeCell ref="A48:A55"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="C32:C35"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="D28:D31"/>
-    <mergeCell ref="E28:E31"/>
-    <mergeCell ref="I36:I39"/>
-    <mergeCell ref="A40:A47"/>
-    <mergeCell ref="B40:B47"/>
-    <mergeCell ref="C40:C47"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="D24:D27"/>
-    <mergeCell ref="E24:E27"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="D20:D23"/>
-    <mergeCell ref="E20:E23"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="C16:C19"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="E16:E19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="I2:I5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="C6:C11"/>
-    <mergeCell ref="D6:D11"/>
-    <mergeCell ref="E6:E11"/>
-    <mergeCell ref="I6:I11"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="I60:I64"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="C78:C82"/>
-    <mergeCell ref="D78:D82"/>
-    <mergeCell ref="E78:E82"/>
-    <mergeCell ref="A65:A69"/>
-    <mergeCell ref="B65:B69"/>
-    <mergeCell ref="C65:C69"/>
-    <mergeCell ref="D65:D69"/>
-    <mergeCell ref="E65:E69"/>
-    <mergeCell ref="I65:I69"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="C70:C74"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="I118:I121"/>
-    <mergeCell ref="A118:A121"/>
-    <mergeCell ref="B118:B121"/>
-    <mergeCell ref="C118:C121"/>
-    <mergeCell ref="D118:D121"/>
-    <mergeCell ref="E118:E121"/>
-    <mergeCell ref="E70:E74"/>
-    <mergeCell ref="I70:I74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="C75:C77"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="E75:E77"/>
-    <mergeCell ref="I75:I77"/>
-    <mergeCell ref="A109:A111"/>
-    <mergeCell ref="B109:B111"/>
-    <mergeCell ref="C109:C111"/>
-    <mergeCell ref="D109:D111"/>
-    <mergeCell ref="E109:E111"/>
-    <mergeCell ref="C92:C97"/>
-    <mergeCell ref="D92:D97"/>
-    <mergeCell ref="E92:E97"/>
-    <mergeCell ref="A98:A102"/>
-    <mergeCell ref="B98:B102"/>
-    <mergeCell ref="A103:A108"/>
-    <mergeCell ref="B103:B108"/>
-    <mergeCell ref="C103:C108"/>
-    <mergeCell ref="D103:D108"/>
-    <mergeCell ref="E103:E108"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="C60:C64"/>
-    <mergeCell ref="D60:D64"/>
-    <mergeCell ref="E60:E64"/>
-    <mergeCell ref="C98:C102"/>
-    <mergeCell ref="D98:D102"/>
-    <mergeCell ref="E98:E102"/>
-    <mergeCell ref="A83:A91"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>